<commit_message>
Updated Monthly Tracker tool to pull Yelp For Help Candidates into surgery report
</commit_message>
<xml_diff>
--- a/Monthly Dept Head Tracking Tool/Department Head Monthly Report Generation.xlsx
+++ b/Monthly Dept Head Tracking Tool/Department Head Monthly Report Generation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="150">
   <si>
     <t>Category</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Others Other Surgeries</t>
+  </si>
+  <si>
+    <t>Yelp For Help Candidate</t>
   </si>
   <si>
     <t>AnimalNumber</t>
@@ -1277,7 +1280,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1385,6 +1388,14 @@
       </c>
       <c r="B16">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1402,870 +1413,870 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C36" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C47" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C48" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C56" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C57" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C58" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B59" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C60" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D60" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B61" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B62" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C62" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D62" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2283,86 +2294,86 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C2" s="2">
         <v>45812.62761574074</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2">
         <v>45814.4284375</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="2">
         <v>45814.64461805556</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C5" s="2">
         <v>45814.67733796296</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C6" s="2">
         <v>45812.62761574074</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2380,19 +2391,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Outcome, Foster, and Veterinary Monthly Data
</commit_message>
<xml_diff>
--- a/Monthly Dept Head Tracking Tool/Department Head Monthly Report Generation.xlsx
+++ b/Monthly Dept Head Tracking Tool/Department Head Monthly Report Generation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="172">
   <si>
     <t>Category</t>
   </si>
@@ -231,187 +231,193 @@
     <t>OperationSubType</t>
   </si>
   <si>
-    <t>A0015599570</t>
-  </si>
-  <si>
-    <t>A0051151112</t>
-  </si>
-  <si>
-    <t>A0052271961</t>
-  </si>
-  <si>
-    <t>A0057052406</t>
-  </si>
-  <si>
-    <t>A0058344428</t>
-  </si>
-  <si>
-    <t>A0058581220</t>
-  </si>
-  <si>
-    <t>A0058588779</t>
-  </si>
-  <si>
-    <t>A0058589089</t>
-  </si>
-  <si>
-    <t>A0058598326</t>
-  </si>
-  <si>
-    <t>A0058612059</t>
-  </si>
-  <si>
-    <t>A0058620400</t>
-  </si>
-  <si>
-    <t>A0058620581</t>
-  </si>
-  <si>
-    <t>A0058621971</t>
-  </si>
-  <si>
-    <t>A0058622243</t>
-  </si>
-  <si>
-    <t>A0058623854</t>
-  </si>
-  <si>
-    <t>A0058623878</t>
-  </si>
-  <si>
-    <t>A0058624438</t>
-  </si>
-  <si>
-    <t>A0058630015</t>
-  </si>
-  <si>
-    <t>A0058640561</t>
-  </si>
-  <si>
-    <t>A0058647055</t>
-  </si>
-  <si>
-    <t>A0058648384</t>
-  </si>
-  <si>
-    <t>A0058655448</t>
-  </si>
-  <si>
-    <t>A0058668717</t>
-  </si>
-  <si>
-    <t>A0058669677</t>
-  </si>
-  <si>
-    <t>A0058670777</t>
-  </si>
-  <si>
-    <t>A0058670929</t>
-  </si>
-  <si>
-    <t>A0058671983</t>
-  </si>
-  <si>
-    <t>A0058672839</t>
-  </si>
-  <si>
-    <t>A0058676198</t>
-  </si>
-  <si>
-    <t>A0058676386</t>
-  </si>
-  <si>
-    <t>A0058686978</t>
-  </si>
-  <si>
-    <t>A0058688511</t>
-  </si>
-  <si>
-    <t>A0058694957</t>
-  </si>
-  <si>
-    <t>A0058702255</t>
-  </si>
-  <si>
-    <t>A0058705115</t>
-  </si>
-  <si>
-    <t>A0058706029</t>
-  </si>
-  <si>
-    <t>A0058709149</t>
-  </si>
-  <si>
-    <t>A0058709460</t>
-  </si>
-  <si>
-    <t>A0058712391</t>
-  </si>
-  <si>
-    <t>A0058717573</t>
-  </si>
-  <si>
-    <t>A0058718599</t>
-  </si>
-  <si>
-    <t>A0058723929</t>
-  </si>
-  <si>
-    <t>A0058727921</t>
-  </si>
-  <si>
-    <t>A0058729123</t>
-  </si>
-  <si>
-    <t>A0058736922</t>
-  </si>
-  <si>
-    <t>A0058737688</t>
-  </si>
-  <si>
-    <t>A0058748113</t>
-  </si>
-  <si>
-    <t>A0058749076</t>
-  </si>
-  <si>
-    <t>A0058755847</t>
-  </si>
-  <si>
-    <t>A0058763044</t>
-  </si>
-  <si>
-    <t>A0058770794</t>
-  </si>
-  <si>
-    <t>A0058771476</t>
-  </si>
-  <si>
-    <t>A0058775218</t>
-  </si>
-  <si>
-    <t>A0058779323</t>
-  </si>
-  <si>
-    <t>A0058779670</t>
-  </si>
-  <si>
-    <t>A0058780847</t>
-  </si>
-  <si>
-    <t>A0058787214</t>
-  </si>
-  <si>
-    <t>A0058789307</t>
-  </si>
-  <si>
-    <t>A0058790320</t>
-  </si>
-  <si>
-    <t>A0058803369</t>
-  </si>
-  <si>
-    <t>A0058804124</t>
+    <t>A0013296738</t>
+  </si>
+  <si>
+    <t>A0021403555</t>
+  </si>
+  <si>
+    <t>A0034433659</t>
+  </si>
+  <si>
+    <t>A0035360496</t>
+  </si>
+  <si>
+    <t>A0049458539</t>
+  </si>
+  <si>
+    <t>A0054633714</t>
+  </si>
+  <si>
+    <t>A0057812734</t>
+  </si>
+  <si>
+    <t>A0057843440</t>
+  </si>
+  <si>
+    <t>A0058258185</t>
+  </si>
+  <si>
+    <t>A0058497276</t>
+  </si>
+  <si>
+    <t>A0058797381</t>
+  </si>
+  <si>
+    <t>A0058819189</t>
+  </si>
+  <si>
+    <t>A0058820045</t>
+  </si>
+  <si>
+    <t>A0058822858</t>
+  </si>
+  <si>
+    <t>A0058828077</t>
+  </si>
+  <si>
+    <t>A0058830603</t>
+  </si>
+  <si>
+    <t>A0058832269</t>
+  </si>
+  <si>
+    <t>A0058836833</t>
+  </si>
+  <si>
+    <t>A0058847033</t>
+  </si>
+  <si>
+    <t>A0058847947</t>
+  </si>
+  <si>
+    <t>A0058854247</t>
+  </si>
+  <si>
+    <t>A0058854337</t>
+  </si>
+  <si>
+    <t>A0058859277</t>
+  </si>
+  <si>
+    <t>A0058863798</t>
+  </si>
+  <si>
+    <t>A0058871910</t>
+  </si>
+  <si>
+    <t>A0058878747</t>
+  </si>
+  <si>
+    <t>A0058878916</t>
+  </si>
+  <si>
+    <t>A0058887134</t>
+  </si>
+  <si>
+    <t>A0058887853</t>
+  </si>
+  <si>
+    <t>A0058894633</t>
+  </si>
+  <si>
+    <t>A0058895660</t>
+  </si>
+  <si>
+    <t>A0058896079</t>
+  </si>
+  <si>
+    <t>A0058901666</t>
+  </si>
+  <si>
+    <t>A0058904051</t>
+  </si>
+  <si>
+    <t>A0058910023</t>
+  </si>
+  <si>
+    <t>A0058919342</t>
+  </si>
+  <si>
+    <t>A0058921180</t>
+  </si>
+  <si>
+    <t>A0058925581</t>
+  </si>
+  <si>
+    <t>A0058925658</t>
+  </si>
+  <si>
+    <t>A0058926055</t>
+  </si>
+  <si>
+    <t>A0058933398</t>
+  </si>
+  <si>
+    <t>A0058933633</t>
+  </si>
+  <si>
+    <t>A0058934219</t>
+  </si>
+  <si>
+    <t>A0058936894</t>
+  </si>
+  <si>
+    <t>A0058937365</t>
+  </si>
+  <si>
+    <t>A0058948528</t>
+  </si>
+  <si>
+    <t>A0058949012</t>
+  </si>
+  <si>
+    <t>A0058951360</t>
+  </si>
+  <si>
+    <t>A0058957705</t>
+  </si>
+  <si>
+    <t>A0058957748</t>
+  </si>
+  <si>
+    <t>A0058964925</t>
+  </si>
+  <si>
+    <t>A0058965883</t>
+  </si>
+  <si>
+    <t>A0058966220</t>
+  </si>
+  <si>
+    <t>A0058971377</t>
+  </si>
+  <si>
+    <t>A0058972377</t>
+  </si>
+  <si>
+    <t>A0058972383</t>
+  </si>
+  <si>
+    <t>A0058973545</t>
+  </si>
+  <si>
+    <t>A0058975230</t>
+  </si>
+  <si>
+    <t>A0058975680</t>
+  </si>
+  <si>
+    <t>A0058979799</t>
+  </si>
+  <si>
+    <t>A0058981340</t>
+  </si>
+  <si>
+    <t>A0059000673</t>
+  </si>
+  <si>
+    <t>A0059002296</t>
   </si>
   <si>
     <t>Cat</t>
@@ -426,6 +432,9 @@
     <t>Rodent</t>
   </si>
   <si>
+    <t>Reptile/Amphibian</t>
+  </si>
+  <si>
     <t>Euthanasia</t>
   </si>
   <si>
@@ -444,24 +453,6 @@
     <t>Foster Start Reason</t>
   </si>
   <si>
-    <t>A0058545042</t>
-  </si>
-  <si>
-    <t>A0058545061</t>
-  </si>
-  <si>
-    <t>A0058545067</t>
-  </si>
-  <si>
-    <t>A0058545079</t>
-  </si>
-  <si>
-    <t>A0058545429</t>
-  </si>
-  <si>
-    <t>Event Hold!</t>
-  </si>
-  <si>
     <t>Record #</t>
   </si>
   <si>
@@ -469,15 +460,87 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>M0083183234</t>
+  </si>
+  <si>
+    <t>M0083204596</t>
+  </si>
+  <si>
+    <t>M0083215311</t>
+  </si>
+  <si>
+    <t>M0083215630</t>
+  </si>
+  <si>
+    <t>M0083278251</t>
+  </si>
+  <si>
+    <t>M0083278252</t>
+  </si>
+  <si>
+    <t>M0083278253</t>
+  </si>
+  <si>
+    <t>M0083278254</t>
+  </si>
+  <si>
+    <t>Spay</t>
+  </si>
+  <si>
+    <t>A0058955676</t>
+  </si>
+  <si>
+    <t>A0058955673</t>
+  </si>
+  <si>
+    <t>A0058955689</t>
+  </si>
+  <si>
+    <t>A0058955731</t>
+  </si>
+  <si>
+    <t>A0058955576</t>
+  </si>
+  <si>
+    <t>A0058955700</t>
+  </si>
+  <si>
+    <t>A0058955706</t>
+  </si>
+  <si>
+    <t>A0058955726</t>
+  </si>
+  <si>
+    <t>AMELIA</t>
+  </si>
+  <si>
+    <t>G Pig 26</t>
+  </si>
+  <si>
+    <t>G Pig 29</t>
+  </si>
+  <si>
+    <t>G Pig 39</t>
+  </si>
+  <si>
+    <t>G Pig 11</t>
+  </si>
+  <si>
+    <t>G Pig 31</t>
+  </si>
+  <si>
+    <t>G Pig 33</t>
+  </si>
+  <si>
+    <t>G Pig 38</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -530,12 +593,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>137</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -857,7 +919,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -873,7 +935,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -881,7 +943,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -897,7 +959,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -905,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -921,7 +983,7 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -993,7 +1055,7 @@
         <v>20</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1001,7 +1063,7 @@
         <v>21</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1017,7 +1079,7 @@
         <v>23</v>
       </c>
       <c r="B30">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1025,7 +1087,7 @@
         <v>24</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1062,7 +1124,7 @@
         <v>26</v>
       </c>
       <c r="B2">
-        <v>82</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1070,7 +1132,7 @@
         <v>27</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1078,7 +1140,7 @@
         <v>28</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1086,7 +1148,7 @@
         <v>29</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1094,7 +1156,7 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1110,7 +1172,7 @@
         <v>32</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1118,7 +1180,7 @@
         <v>33</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1134,7 +1196,7 @@
         <v>35</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1150,7 +1212,7 @@
         <v>37</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1158,7 +1220,7 @@
         <v>38</v>
       </c>
       <c r="B15">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1166,7 +1228,7 @@
         <v>39</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1174,7 +1236,7 @@
         <v>40</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1190,7 +1252,7 @@
         <v>42</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1206,7 +1268,7 @@
         <v>44</v>
       </c>
       <c r="B22">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1222,7 +1284,7 @@
         <v>46</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1230,7 +1292,7 @@
         <v>47</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1238,7 +1300,7 @@
         <v>48</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1254,7 +1316,7 @@
         <v>50</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1299,7 +1361,7 @@
         <v>53</v>
       </c>
       <c r="B2">
-        <v>69</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1307,7 +1369,7 @@
         <v>54</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1315,7 +1377,7 @@
         <v>55</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1323,7 +1385,7 @@
         <v>56</v>
       </c>
       <c r="B6">
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1331,7 +1393,7 @@
         <v>57</v>
       </c>
       <c r="B7">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1339,7 +1401,7 @@
         <v>58</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1355,7 +1417,7 @@
         <v>60</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1363,7 +1425,7 @@
         <v>61</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1371,7 +1433,7 @@
         <v>62</v>
       </c>
       <c r="B14">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1379,7 +1441,7 @@
         <v>63</v>
       </c>
       <c r="B15">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1395,7 +1457,7 @@
         <v>65</v>
       </c>
       <c r="B18">
-        <v>58</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1405,7 +1467,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1430,13 +1492,13 @@
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1444,13 +1506,13 @@
         <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1458,13 +1520,13 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1472,13 +1534,13 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1486,13 +1548,13 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1500,13 +1562,13 @@
         <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1517,10 +1579,10 @@
         <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1528,13 +1590,13 @@
         <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1542,13 +1604,13 @@
         <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1556,13 +1618,13 @@
         <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1570,13 +1632,13 @@
         <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1584,13 +1646,13 @@
         <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1598,13 +1660,13 @@
         <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1612,13 +1674,13 @@
         <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1626,13 +1688,13 @@
         <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1643,10 +1705,10 @@
         <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1654,13 +1716,13 @@
         <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1668,13 +1730,13 @@
         <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1682,13 +1744,13 @@
         <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1696,13 +1758,13 @@
         <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1710,13 +1772,13 @@
         <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1724,13 +1786,13 @@
         <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C23" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1738,13 +1800,13 @@
         <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1752,13 +1814,13 @@
         <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1766,13 +1828,13 @@
         <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1780,13 +1842,13 @@
         <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D27" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1794,13 +1856,13 @@
         <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1808,13 +1870,13 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1822,13 +1884,13 @@
         <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C30" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1836,13 +1898,13 @@
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1850,13 +1912,13 @@
         <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1864,13 +1926,13 @@
         <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1878,13 +1940,13 @@
         <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1892,13 +1954,13 @@
         <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1906,13 +1968,13 @@
         <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1920,13 +1982,13 @@
         <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1934,13 +1996,13 @@
         <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1948,13 +2010,13 @@
         <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1962,13 +2024,13 @@
         <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1976,13 +2038,13 @@
         <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1990,13 +2052,13 @@
         <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2004,13 +2066,13 @@
         <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C43" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2018,13 +2080,13 @@
         <v>112</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2032,13 +2094,13 @@
         <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C45" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2046,13 +2108,13 @@
         <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2060,13 +2122,13 @@
         <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2074,13 +2136,13 @@
         <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C48" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D48" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2088,13 +2150,13 @@
         <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C49" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2102,13 +2164,13 @@
         <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2116,13 +2178,13 @@
         <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2130,13 +2192,13 @@
         <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2144,13 +2206,13 @@
         <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2161,10 +2223,10 @@
         <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2172,13 +2234,13 @@
         <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2186,13 +2248,13 @@
         <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2200,13 +2262,13 @@
         <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2214,13 +2276,13 @@
         <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C58" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2228,13 +2290,13 @@
         <v>127</v>
       </c>
       <c r="B59" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2242,13 +2304,13 @@
         <v>128</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C60" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D60" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2256,13 +2318,13 @@
         <v>129</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D61" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2270,13 +2332,41 @@
         <v>130</v>
       </c>
       <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
         <v>131</v>
       </c>
-      <c r="C62" t="s">
-        <v>135</v>
-      </c>
-      <c r="D62" t="s">
-        <v>136</v>
+      <c r="B63" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" t="s">
+        <v>138</v>
+      </c>
+      <c r="D63" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>132</v>
+      </c>
+      <c r="B64" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2286,7 +2376,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2294,86 +2384,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45812.62761574074</v>
-      </c>
-      <c r="D2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45814.4284375</v>
-      </c>
-      <c r="D3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
         <v>143</v>
-      </c>
-      <c r="B4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45814.64461805556</v>
-      </c>
-      <c r="D4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45814.67733796296</v>
-      </c>
-      <c r="D5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45812.62761574074</v>
-      </c>
-      <c r="D6" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2383,7 +2403,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2391,19 +2411,155 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>149</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>